<commit_message>
update datasets and predictions
</commit_message>
<xml_diff>
--- a/reports/predictions.xlsx
+++ b/reports/predictions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BB5"/>
+  <dimension ref="A1:BB3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -708,33 +708,33 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Gainsborough</t>
+          <t>Al Urooba</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hyde Utd</t>
+          <t>Gulf United FC</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>4.431983762541822</v>
+        <v>5.817372040222314</v>
       </c>
       <c r="D2" t="n">
-        <v>3.939541122259397</v>
+        <v>4.114001329649735</v>
       </c>
       <c r="E2" t="n">
-        <v>8.37152488480122</v>
+        <v>9.931373369872048</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>draw</t>
+          <t>home</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>4.5</v>
+        <v>6.384615384615385</v>
       </c>
       <c r="H2" t="n">
-        <v>4</v>
+        <v>4.515151515151516</v>
       </c>
       <c r="I2" t="n">
         <v>1</v>
@@ -755,16 +755,16 @@
         <v>9.5</v>
       </c>
       <c r="O2" t="n">
-        <v>0.9848852805648494</v>
+        <v>0.9111546569022901</v>
       </c>
       <c r="P2" t="n">
-        <v>1.85267397592867</v>
+        <v>1.422212949140956</v>
       </c>
       <c r="Q2" t="n">
-        <v>6.673344794024461</v>
+        <v>8.264910242103642</v>
       </c>
       <c r="R2" t="n">
-        <v>2.529150146811159</v>
+        <v>3.833224586029568</v>
       </c>
       <c r="S2" t="inlineStr">
         <is>
@@ -772,19 +772,19 @@
         </is>
       </c>
       <c r="T2" t="n">
-        <v>1.5948</v>
+        <v>1.27</v>
       </c>
       <c r="U2" t="n">
-        <v>2.89</v>
+        <v>2.4342</v>
       </c>
       <c r="V2" t="n">
-        <v>4.2</v>
+        <v>3.08</v>
       </c>
       <c r="W2" t="n">
-        <v>1.28</v>
+        <v>1.22</v>
       </c>
       <c r="X2" t="n">
-        <v>1.1</v>
+        <v>1.06</v>
       </c>
       <c r="Y2" t="inlineStr">
         <is>
@@ -792,123 +792,123 @@
         </is>
       </c>
       <c r="Z2" t="n">
-        <v>2.2024</v>
+        <v>3.43</v>
       </c>
       <c r="AA2" t="n">
-        <v>3.3</v>
+        <v>3.85</v>
       </c>
       <c r="AB2" t="n">
-        <v>5.78</v>
+        <v>7.12</v>
       </c>
       <c r="AC2" t="n">
-        <v>1.36</v>
+        <v>1.4919</v>
       </c>
       <c r="AD2" t="n">
-        <v>1.19</v>
+        <v>1.32</v>
       </c>
       <c r="AE2" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>2.72</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>1.713</v>
+      </c>
+      <c r="AH2" t="n">
         <v>2.0109</v>
       </c>
-      <c r="AF2" t="n">
-        <v>1.713</v>
-      </c>
-      <c r="AG2" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="AH2" t="n">
-        <v>1.38</v>
-      </c>
       <c r="AI2" t="n">
-        <v>4.2</v>
+        <v>2.2561</v>
       </c>
       <c r="AJ2" t="n">
-        <v>1.19</v>
+        <v>1.5678</v>
       </c>
       <c r="AK2" t="n">
-        <v>6.61</v>
+        <v>3.08</v>
       </c>
       <c r="AL2" t="n">
-        <v>1.08</v>
+        <v>1.32</v>
       </c>
       <c r="AM2" t="n">
-        <v>1.42</v>
+        <v>1.11</v>
       </c>
       <c r="AN2" t="n">
-        <v>2.64</v>
+        <v>5.44</v>
       </c>
       <c r="AO2" t="n">
-        <v>2.0109</v>
+        <v>1.34</v>
       </c>
       <c r="AP2" t="n">
-        <v>1.713</v>
+        <v>2.98</v>
       </c>
       <c r="AQ2" t="n">
-        <v>3.19</v>
+        <v>1.7453</v>
       </c>
       <c r="AR2" t="n">
-        <v>1.3</v>
+        <v>1.9681</v>
       </c>
       <c r="AS2" t="n">
-        <v>5.78</v>
+        <v>2.5</v>
       </c>
       <c r="AT2" t="n">
-        <v>1.1</v>
+        <v>1.4683</v>
       </c>
       <c r="AU2" t="n">
-        <v>1.6518</v>
+        <v>1.5678</v>
       </c>
       <c r="AV2" t="n">
-        <v>2.1023</v>
+        <v>2.2561</v>
       </c>
       <c r="AW2" t="n">
-        <v>2.5694</v>
+        <v>2.3718</v>
       </c>
       <c r="AX2" t="n">
-        <v>1.4453</v>
+        <v>1.5164</v>
       </c>
       <c r="AY2" t="n">
-        <v>4.4</v>
+        <v>4.02</v>
       </c>
       <c r="AZ2" t="n">
-        <v>1.17</v>
+        <v>1.2</v>
       </c>
       <c r="BA2" t="n">
-        <v>8.41</v>
+        <v>7.71</v>
       </c>
       <c r="BB2" t="n">
-        <v>1.04</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Prescot Cables</t>
+          <t>Al Arabi Umm Al Quwain</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Warrington Rylands</t>
+          <t>Masfout CSC</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>4.313384943298114</v>
+        <v>3.890982603479163</v>
       </c>
       <c r="D3" t="n">
-        <v>4.930825126713771</v>
+        <v>3.701800345861729</v>
       </c>
       <c r="E3" t="n">
-        <v>9.244210070011885</v>
+        <v>7.592782949340892</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>away</t>
+          <t>draw</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>4.592592592592593</v>
+        <v>3.741935483870968</v>
       </c>
       <c r="H3" t="n">
-        <v>5.25</v>
+        <v>3.56</v>
       </c>
       <c r="I3" t="n">
         <v>1</v>
@@ -929,16 +929,16 @@
         <v>9.5</v>
       </c>
       <c r="O3" t="n">
-        <v>0.9392047860407182</v>
+        <v>1.039831557826328</v>
       </c>
       <c r="P3" t="n">
-        <v>2.594654740093986</v>
+        <v>2.033052158424792</v>
       </c>
       <c r="Q3" t="n">
-        <v>7.062120509450922</v>
+        <v>6.270910960090922</v>
       </c>
       <c r="R3" t="n">
-        <v>1.792141228987031</v>
+        <v>2.305942064849758</v>
       </c>
       <c r="S3" t="inlineStr">
         <is>
@@ -946,458 +946,110 @@
         </is>
       </c>
       <c r="T3" t="n">
-        <v>2.2561</v>
+        <v>1.7453</v>
       </c>
       <c r="U3" t="n">
+        <v>3.08</v>
+      </c>
+      <c r="V3" t="n">
+        <v>4.87</v>
+      </c>
+      <c r="W3" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="X3" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>2-я команда (Гости)</t>
+        </is>
+      </c>
+      <c r="Z3" t="n">
+        <v>1.9681</v>
+      </c>
+      <c r="AA3" t="n">
         <v>3.3</v>
       </c>
-      <c r="V3" t="n">
+      <c r="AB3" t="n">
         <v>5.44</v>
       </c>
-      <c r="W3" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="X3" t="n">
+      <c r="AC3" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>2.64</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>3.85</v>
+      </c>
+      <c r="AH3" t="n">
         <v>1.22</v>
       </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>2-я команда (Гости)</t>
-        </is>
-      </c>
-      <c r="Z3" t="n">
-        <v>1.5678</v>
-      </c>
-      <c r="AA3" t="n">
-        <v>2.72</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>3.85</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>1.28</v>
-      </c>
-      <c r="AD3" t="n">
+      <c r="AI3" t="n">
+        <v>6.17</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>10.28</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>1.6818</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>2.0556</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>2.64</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>4.63</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>9.25</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>1.8137</v>
+      </c>
+      <c r="AV3" t="n">
+        <v>1.8878</v>
+      </c>
+      <c r="AW3" t="n">
+        <v>2.98</v>
+      </c>
+      <c r="AX3" t="n">
+        <v>1.34</v>
+      </c>
+      <c r="AY3" t="n">
+        <v>5.44</v>
+      </c>
+      <c r="AZ3" t="n">
         <v>1.11</v>
       </c>
-      <c r="AE3" t="n">
-        <v>1.5948</v>
-      </c>
-      <c r="AF3" t="n">
-        <v>2.2024</v>
-      </c>
-      <c r="AG3" t="n">
-        <v>2.0556</v>
-      </c>
-      <c r="AH3" t="n">
-        <v>1.6818</v>
-      </c>
-      <c r="AI3" t="n">
-        <v>2.89</v>
-      </c>
-      <c r="AJ3" t="n">
-        <v>1.36</v>
-      </c>
-      <c r="AK3" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="AL3" t="n">
-        <v>1.19</v>
-      </c>
-      <c r="AM3" t="n">
-        <v>1.4683</v>
-      </c>
-      <c r="AN3" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="AO3" t="n">
-        <v>2.1512</v>
-      </c>
-      <c r="AP3" t="n">
-        <v>1.6228</v>
-      </c>
-      <c r="AQ3" t="n">
-        <v>3.43</v>
-      </c>
-      <c r="AR3" t="n">
-        <v>1.27</v>
-      </c>
-      <c r="AS3" t="n">
-        <v>6.17</v>
-      </c>
-      <c r="AT3" t="n">
-        <v>1.09</v>
-      </c>
-      <c r="AU3" t="n">
-        <v>1.27</v>
-      </c>
-      <c r="AV3" t="n">
-        <v>3.43</v>
-      </c>
-      <c r="AW3" t="n">
-        <v>1.6818</v>
-      </c>
-      <c r="AX3" t="n">
-        <v>2.0556</v>
-      </c>
-      <c r="AY3" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="AZ3" t="n">
-        <v>1.4683</v>
-      </c>
       <c r="BA3" t="n">
-        <v>4.02</v>
+        <v>11.56</v>
       </c>
       <c r="BB3" t="n">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>FC United of Manchester</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Stockton Town</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>5.154259543667063</v>
-      </c>
-      <c r="D4" t="n">
-        <v>4.72632606222647</v>
-      </c>
-      <c r="E4" t="n">
-        <v>9.880585605893533</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>draw</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>5.645161290322581</v>
-      </c>
-      <c r="H4" t="n">
-        <v>5.176470588235294</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" t="n">
-        <v>1</v>
-      </c>
-      <c r="L4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N4" t="n">
-        <v>9.5</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0.9130402620210225</v>
-      </c>
-      <c r="P4" t="n">
-        <v>1.882381914798903</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>7.22393863004072</v>
-      </c>
-      <c r="R4" t="n">
-        <v>2.407726662599487</v>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>1-я команда (Дома)</t>
-        </is>
-      </c>
-      <c r="T4" t="n">
-        <v>1.6518</v>
-      </c>
-      <c r="U4" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="V4" t="n">
-        <v>4.02</v>
-      </c>
-      <c r="W4" t="n">
-        <v>1.32</v>
-      </c>
-      <c r="X4" t="n">
-        <v>1.14</v>
-      </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>2-я команда (Гости)</t>
-        </is>
-      </c>
-      <c r="Z4" t="n">
-        <v>2.1023</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>3.08</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>4.87</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>1.38</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>1.42</v>
-      </c>
-      <c r="AF4" t="n">
-        <v>2.64</v>
-      </c>
-      <c r="AG4" t="n">
-        <v>1.7453</v>
-      </c>
-      <c r="AH4" t="n">
-        <v>1.9681</v>
-      </c>
-      <c r="AI4" t="n">
-        <v>2.3125</v>
-      </c>
-      <c r="AJ4" t="n">
-        <v>1.5417</v>
-      </c>
-      <c r="AK4" t="n">
-        <v>3.19</v>
-      </c>
-      <c r="AL4" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="AM4" t="n">
-        <v>1.22</v>
-      </c>
-      <c r="AN4" t="n">
-        <v>3.85</v>
-      </c>
-      <c r="AO4" t="n">
-        <v>1.5678</v>
-      </c>
-      <c r="AP4" t="n">
-        <v>2.2561</v>
-      </c>
-      <c r="AQ4" t="n">
-        <v>2.2561</v>
-      </c>
-      <c r="AR4" t="n">
-        <v>1.5678</v>
-      </c>
-      <c r="AS4" t="n">
-        <v>3.56</v>
-      </c>
-      <c r="AT4" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="AU4" t="n">
-        <v>1.32</v>
-      </c>
-      <c r="AV4" t="n">
-        <v>3.08</v>
-      </c>
-      <c r="AW4" t="n">
-        <v>1.8137</v>
-      </c>
-      <c r="AX4" t="n">
-        <v>1.8878</v>
-      </c>
-      <c r="AY4" t="n">
-        <v>2.72</v>
-      </c>
-      <c r="AZ4" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="BA4" t="n">
-        <v>4.63</v>
-      </c>
-      <c r="BB4" t="n">
-        <v>1.16</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Cleethorpes Town</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Whitby</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>5.047802447645457</v>
-      </c>
-      <c r="D5" t="n">
-        <v>3.457055770595896</v>
-      </c>
-      <c r="E5" t="n">
-        <v>8.504858218241353</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>home</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>5.166666666666667</v>
-      </c>
-      <c r="H5" t="n">
-        <v>3.538461538461538</v>
-      </c>
-      <c r="I5" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" t="n">
-        <v>1</v>
-      </c>
-      <c r="L5" t="n">
-        <v>1</v>
-      </c>
-      <c r="M5" t="n">
-        <v>1</v>
-      </c>
-      <c r="N5" t="n">
-        <v>9.5</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0.9769940221249271</v>
-      </c>
-      <c r="P5" t="n">
-        <v>1.42940601586191</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>7.630410623069879</v>
-      </c>
-      <c r="R5" t="n">
-        <v>3.931525980174345</v>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>1-я команда (Дома)</t>
-        </is>
-      </c>
-      <c r="T5" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="U5" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="V5" t="n">
-        <v>3.19</v>
-      </c>
-      <c r="W5" t="n">
-        <v>1.19</v>
-      </c>
-      <c r="X5" t="n">
-        <v>1.04</v>
-      </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>2-я команда (Гости)</t>
-        </is>
-      </c>
-      <c r="Z5" t="n">
-        <v>3.56</v>
-      </c>
-      <c r="AA5" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="AB5" t="n">
-        <v>8.41</v>
-      </c>
-      <c r="AC5" t="n">
-        <v>1.4683</v>
-      </c>
-      <c r="AD5" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="AE5" t="n">
-        <v>1.9271</v>
-      </c>
-      <c r="AF5" t="n">
-        <v>1.7788</v>
-      </c>
-      <c r="AG5" t="n">
-        <v>2.64</v>
-      </c>
-      <c r="AH5" t="n">
-        <v>1.42</v>
-      </c>
-      <c r="AI5" t="n">
-        <v>3.85</v>
-      </c>
-      <c r="AJ5" t="n">
-        <v>1.22</v>
-      </c>
-      <c r="AK5" t="n">
-        <v>6.17</v>
-      </c>
-      <c r="AL5" t="n">
-        <v>1.09</v>
-      </c>
-      <c r="AM5" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="AN5" t="n">
-        <v>3.56</v>
-      </c>
-      <c r="AO5" t="n">
-        <v>1.6228</v>
-      </c>
-      <c r="AP5" t="n">
-        <v>2.1512</v>
-      </c>
-      <c r="AQ5" t="n">
-        <v>2.3718</v>
-      </c>
-      <c r="AR5" t="n">
-        <v>1.5164</v>
-      </c>
-      <c r="AS5" t="n">
-        <v>3.7</v>
-      </c>
-      <c r="AT5" t="n">
-        <v>1.23</v>
-      </c>
-      <c r="AU5" t="n">
-        <v>2.0109</v>
-      </c>
-      <c r="AV5" t="n">
-        <v>1.713</v>
-      </c>
-      <c r="AW5" t="n">
-        <v>3.43</v>
-      </c>
-      <c r="AX5" t="n">
-        <v>1.27</v>
-      </c>
-      <c r="AY5" t="n">
-        <v>6.61</v>
-      </c>
-      <c r="AZ5" t="n">
-        <v>1.08</v>
-      </c>
-      <c r="BA5" t="n">
-        <v>11.56</v>
-      </c>
-      <c r="BB5" t="n">
         <v>1.01</v>
       </c>
     </row>

</xml_diff>